<commit_message>
comparison done for k=32
</commit_message>
<xml_diff>
--- a/Code/results/testing.xlsx
+++ b/Code/results/testing.xlsx
@@ -426,7 +426,7 @@
   <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1208,6 +1208,15 @@
       <c r="D28">
         <v>0.5</v>
       </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <v>16</v>
+      </c>
+      <c r="G28">
+        <v>0.45</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29">
@@ -1218,6 +1227,15 @@
       </c>
       <c r="D29">
         <v>0.6</v>
+      </c>
+      <c r="E29">
+        <v>7</v>
+      </c>
+      <c r="F29">
+        <v>32</v>
+      </c>
+      <c r="G29">
+        <v>0.41</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
@@ -1230,6 +1248,15 @@
       <c r="D30">
         <v>0.52</v>
       </c>
+      <c r="E30">
+        <v>7</v>
+      </c>
+      <c r="F30">
+        <v>32</v>
+      </c>
+      <c r="G30">
+        <v>0.39</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31">
@@ -1241,6 +1268,15 @@
       <c r="D31">
         <v>0.38</v>
       </c>
+      <c r="E31">
+        <v>9</v>
+      </c>
+      <c r="F31">
+        <v>64</v>
+      </c>
+      <c r="G31">
+        <v>0.34</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B32">
@@ -1252,8 +1288,17 @@
       <c r="D32">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>18</v>
+      </c>
+      <c r="F32">
+        <v>256</v>
+      </c>
+      <c r="G32">
+        <v>0.32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>1024</v>
       </c>
@@ -1262,6 +1307,15 @@
       </c>
       <c r="D33">
         <v>0.34</v>
+      </c>
+      <c r="E33">
+        <v>25</v>
+      </c>
+      <c r="F33">
+        <v>512</v>
+      </c>
+      <c r="G33">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
did FJLT 2 for d = 64
</commit_message>
<xml_diff>
--- a/Code/results/testing.xlsx
+++ b/Code/results/testing.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devin\Desktop\FYP\Code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12690" windowHeight="9885"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12690" windowHeight="9885" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
   <si>
     <t>n</t>
   </si>
@@ -63,6 +64,12 @@
   </si>
   <si>
     <t>FJLT 2</t>
+  </si>
+  <si>
+    <t>d^(1/3)</t>
+  </si>
+  <si>
+    <t>d^(1/2)</t>
   </si>
 </sst>
 </file>
@@ -106,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,7 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -1322,4 +1330,117 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>32</v>
+      </c>
+      <c r="B3" s="2">
+        <f>A3^(1/3)</f>
+        <v>3.1748021039363987</v>
+      </c>
+      <c r="C3" s="2">
+        <f>SQRT(A3)</f>
+        <v>5.6568542494923806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>64</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:B8" si="0">A4^(1/3)</f>
+        <v>3.9999999999999991</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C8" si="1">SQRT(A4)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>128</v>
+      </c>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
+        <v>5.0396841995794919</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="1"/>
+        <v>11.313708498984761</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>256</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
+        <v>6.3496042078727974</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>512</v>
+      </c>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>7.9999999999999982</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="1"/>
+        <v>22.627416997969522</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1024</v>
+      </c>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>10.079368399158986</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finals for the report
</commit_message>
<xml_diff>
--- a/Code/results/testing.xlsx
+++ b/Code/results/testing.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12690" windowHeight="9885" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12690" windowHeight="9885"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V33"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G33" sqref="G3:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +536,7 @@
       <c r="C3">
         <v>3</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>0.4</v>
       </c>
       <c r="E3">
@@ -545,7 +545,7 @@
       <c r="F3">
         <v>16</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>0.4</v>
       </c>
       <c r="K3">
@@ -568,7 +568,7 @@
       <c r="C4">
         <v>4</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.44</v>
       </c>
       <c r="E4">
@@ -577,8 +577,8 @@
       <c r="F4">
         <v>32</v>
       </c>
-      <c r="G4">
-        <v>3</v>
+      <c r="G4" s="2">
+        <v>0.38</v>
       </c>
       <c r="L4">
         <v>8</v>
@@ -597,7 +597,7 @@
       <c r="C5">
         <v>4</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.4</v>
       </c>
       <c r="E5">
@@ -606,7 +606,7 @@
       <c r="F5">
         <v>32</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>0.35</v>
       </c>
       <c r="L5">
@@ -626,7 +626,7 @@
       <c r="C6">
         <v>8</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.32</v>
       </c>
       <c r="E6">
@@ -635,7 +635,7 @@
       <c r="F6">
         <v>64</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>0.25</v>
       </c>
       <c r="K6">
@@ -658,7 +658,7 @@
       <c r="C7">
         <v>16</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.3</v>
       </c>
       <c r="E7">
@@ -667,7 +667,7 @@
       <c r="F7">
         <v>256</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>0.25</v>
       </c>
       <c r="L7">
@@ -690,7 +690,7 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>0.5</v>
       </c>
       <c r="E8">
@@ -699,7 +699,7 @@
       <c r="F8">
         <v>16</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>0.38</v>
       </c>
       <c r="L8">
@@ -719,7 +719,7 @@
       <c r="C9">
         <v>3</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.4</v>
       </c>
       <c r="E9">
@@ -728,7 +728,7 @@
       <c r="F9">
         <v>32</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>0.37</v>
       </c>
       <c r="L9">
@@ -748,7 +748,7 @@
       <c r="C10">
         <v>4</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0.4</v>
       </c>
       <c r="E10">
@@ -757,7 +757,7 @@
       <c r="F10">
         <v>32</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>0.34</v>
       </c>
       <c r="K10">
@@ -780,7 +780,7 @@
       <c r="C11">
         <v>8</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.32</v>
       </c>
       <c r="E11">
@@ -789,7 +789,7 @@
       <c r="F11">
         <v>128</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>0.34</v>
       </c>
       <c r="L11">
@@ -809,7 +809,7 @@
       <c r="C12">
         <v>8</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>0.36</v>
       </c>
       <c r="E12">
@@ -818,7 +818,7 @@
       <c r="F12">
         <v>256</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>0.28000000000000003</v>
       </c>
       <c r="L12">
@@ -841,7 +841,7 @@
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>0.52</v>
       </c>
       <c r="E13">
@@ -850,7 +850,7 @@
       <c r="F13">
         <v>16</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>0.42</v>
       </c>
       <c r="L13">
@@ -870,7 +870,7 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0.5</v>
       </c>
       <c r="E14">
@@ -879,7 +879,7 @@
       <c r="F14">
         <v>32</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>0.4</v>
       </c>
       <c r="L14">
@@ -899,7 +899,7 @@
       <c r="C15">
         <v>3</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>0.44</v>
       </c>
       <c r="E15">
@@ -908,7 +908,7 @@
       <c r="F15">
         <v>32</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>0.37</v>
       </c>
       <c r="K15">
@@ -925,7 +925,7 @@
       <c r="C16">
         <v>4</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="2">
         <v>0.4</v>
       </c>
       <c r="E16">
@@ -934,7 +934,7 @@
       <c r="F16">
         <v>64</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>0.35</v>
       </c>
       <c r="L16">
@@ -948,7 +948,7 @@
       <c r="C17">
         <v>8</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="2">
         <v>0.3</v>
       </c>
       <c r="E17">
@@ -957,7 +957,7 @@
       <c r="F17">
         <v>256</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>0.32</v>
       </c>
       <c r="L17">
@@ -974,7 +974,7 @@
       <c r="C18">
         <v>2</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>4.8</v>
       </c>
       <c r="E18">
@@ -983,7 +983,7 @@
       <c r="F18">
         <v>16</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>0.46</v>
       </c>
       <c r="L18">
@@ -997,7 +997,7 @@
       <c r="C19">
         <v>2</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="2">
         <v>0.54</v>
       </c>
       <c r="E19">
@@ -1006,7 +1006,7 @@
       <c r="F19">
         <v>32</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>0.41</v>
       </c>
       <c r="L19">
@@ -1020,7 +1020,7 @@
       <c r="C20">
         <v>4</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="2">
         <v>0.38</v>
       </c>
       <c r="E20">
@@ -1029,7 +1029,7 @@
       <c r="F20">
         <v>32</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>0.38</v>
       </c>
       <c r="L20">
@@ -1043,7 +1043,7 @@
       <c r="C21">
         <v>4</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="2">
         <v>0.4</v>
       </c>
       <c r="E21">
@@ -1052,7 +1052,7 @@
       <c r="F21">
         <v>64</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>0.35</v>
       </c>
       <c r="K21">
@@ -1069,7 +1069,7 @@
       <c r="C22">
         <v>8</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="2">
         <v>0.38</v>
       </c>
       <c r="E22">
@@ -1078,7 +1078,7 @@
       <c r="F22">
         <v>256</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="2">
         <v>0.33</v>
       </c>
       <c r="L22">
@@ -1095,7 +1095,7 @@
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="2">
         <v>0.57999999999999996</v>
       </c>
       <c r="E23">
@@ -1104,7 +1104,7 @@
       <c r="F23">
         <v>16</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="2">
         <v>0.45</v>
       </c>
       <c r="L23">
@@ -1118,7 +1118,7 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>0.46</v>
       </c>
       <c r="E24">
@@ -1127,7 +1127,7 @@
       <c r="F24">
         <v>32</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>0.42</v>
       </c>
       <c r="L24">
@@ -1141,7 +1141,7 @@
       <c r="C25">
         <v>3</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>0.5</v>
       </c>
       <c r="E25">
@@ -1150,7 +1150,7 @@
       <c r="F25">
         <v>32</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>0.39</v>
       </c>
       <c r="L25">
@@ -1164,7 +1164,7 @@
       <c r="C26">
         <v>3</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>0.38</v>
       </c>
       <c r="E26">
@@ -1173,7 +1173,7 @@
       <c r="F26">
         <v>64</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>0.35</v>
       </c>
       <c r="L26">
@@ -1187,7 +1187,7 @@
       <c r="C27">
         <v>4</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>0.36</v>
       </c>
       <c r="E27">
@@ -1196,7 +1196,7 @@
       <c r="F27">
         <v>256</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <v>0.33</v>
       </c>
       <c r="L27">
@@ -1213,7 +1213,7 @@
       <c r="C28">
         <v>2</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>0.5</v>
       </c>
       <c r="E28">
@@ -1222,7 +1222,7 @@
       <c r="F28">
         <v>16</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="2">
         <v>0.45</v>
       </c>
     </row>
@@ -1233,7 +1233,7 @@
       <c r="C29">
         <v>2</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>0.6</v>
       </c>
       <c r="E29">
@@ -1242,7 +1242,7 @@
       <c r="F29">
         <v>32</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="2">
         <v>0.41</v>
       </c>
     </row>
@@ -1253,7 +1253,7 @@
       <c r="C30">
         <v>2</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>0.52</v>
       </c>
       <c r="E30">
@@ -1262,7 +1262,7 @@
       <c r="F30">
         <v>32</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <v>0.39</v>
       </c>
     </row>
@@ -1273,7 +1273,7 @@
       <c r="C31">
         <v>3</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>0.38</v>
       </c>
       <c r="E31">
@@ -1282,7 +1282,7 @@
       <c r="F31">
         <v>64</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="2">
         <v>0.34</v>
       </c>
     </row>
@@ -1293,7 +1293,7 @@
       <c r="C32">
         <v>4</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>0.36</v>
       </c>
       <c r="E32">
@@ -1302,7 +1302,7 @@
       <c r="F32">
         <v>256</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2">
         <v>0.32</v>
       </c>
     </row>
@@ -1313,7 +1313,7 @@
       <c r="C33">
         <v>8</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>0.34</v>
       </c>
       <c r="E33">
@@ -1322,7 +1322,7 @@
       <c r="F33">
         <v>512</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2">
         <v>0.3</v>
       </c>
     </row>
@@ -1336,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>

</xml_diff>